<commit_message>
Update PV and STC data
</commit_message>
<xml_diff>
--- a/realization_times.xlsx
+++ b/realization_times.xlsx
@@ -905,7 +905,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="171" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -1149,6 +1149,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1203,8 +1205,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1797,26 +1797,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>199</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
     </row>
     <row r="2" spans="1:7" ht="69.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="30" t="s">
         <v>198</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="37"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="39"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
@@ -1908,7 +1908,7 @@
         <v>166</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="43">
+      <c r="F7" s="25">
         <v>8.6666666666666661</v>
       </c>
       <c r="G7" s="2"/>
@@ -1929,7 +1929,7 @@
       <c r="E8" s="2">
         <v>4</v>
       </c>
-      <c r="F8" s="43">
+      <c r="F8" s="25">
         <v>5.6000000000000005</v>
       </c>
       <c r="G8" s="2">
@@ -1952,7 +1952,7 @@
       <c r="E9" s="2">
         <v>4</v>
       </c>
-      <c r="F9" s="44">
+      <c r="F9" s="26">
         <v>6</v>
       </c>
       <c r="G9" s="2">
@@ -1973,7 +1973,7 @@
         <v>166</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="44">
+      <c r="F10" s="26">
         <v>8</v>
       </c>
       <c r="G10" s="2">
@@ -1996,7 +1996,7 @@
       <c r="E11" s="2">
         <v>1.8</v>
       </c>
-      <c r="F11" s="43">
+      <c r="F11" s="25">
         <v>2.4333333333333331</v>
       </c>
       <c r="G11" s="2">
@@ -2131,26 +2131,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>231</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
     </row>
     <row r="2" spans="1:7" ht="55.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="30" t="s">
         <v>179</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="30"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="32"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
@@ -2348,25 +2348,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>201</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" ht="19.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="40" t="s">
         <v>200</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -2697,24 +2697,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>203</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
     </row>
     <row r="2" spans="1:6" ht="19.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="40" t="s">
         <v>202</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
@@ -3083,22 +3083,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>205</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="41" t="s">
         <v>204</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
@@ -3365,26 +3365,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>206</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" ht="33.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="41" t="s">
         <v>207</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
@@ -3539,22 +3539,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>209</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="41" t="s">
         <v>208</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
@@ -3838,22 +3838,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>211</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:5" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="41" t="s">
         <v>210</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
@@ -4118,22 +4118,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:5" ht="67.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="41" t="s">
         <v>212</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
@@ -4400,22 +4400,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>215</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:5" ht="76.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="41" t="s">
         <v>214</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
@@ -4652,8 +4652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4663,22 +4663,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>260</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:5" s="2" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="28" t="s">
         <v>261</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
     </row>
     <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A3" s="19" t="s">
@@ -4923,13 +4923,13 @@
         <v>249</v>
       </c>
       <c r="B17">
-        <v>8.5299999999999994</v>
+        <v>4.5</v>
       </c>
       <c r="C17">
-        <v>12.3</v>
+        <v>5.69</v>
       </c>
       <c r="D17">
-        <v>16.7</v>
+        <v>6.99</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>268</v>
@@ -4940,13 +4940,13 @@
         <v>250</v>
       </c>
       <c r="B18">
-        <v>15.6</v>
+        <v>6.76</v>
       </c>
       <c r="C18">
-        <v>23.3</v>
+        <v>8.8699999999999992</v>
       </c>
       <c r="D18">
-        <v>31.2</v>
+        <v>11.05</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>268</v>
@@ -5143,22 +5143,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>217</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:5" ht="71.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="41" t="s">
         <v>216</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
@@ -5306,22 +5306,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>219</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:5" ht="74.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="41" t="s">
         <v>218</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
@@ -5536,22 +5536,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>221</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:5" ht="78.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="41" t="s">
         <v>220</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
@@ -5903,22 +5903,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>180</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:5" ht="85.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="41" t="s">
         <v>230</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
@@ -6099,24 +6099,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>223</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
     </row>
     <row r="2" spans="1:9" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="41" t="s">
         <v>222</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
@@ -6362,8 +6362,8 @@
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="42"/>
-      <c r="B14" s="42"/>
+      <c r="A14" s="44"/>
+      <c r="B14" s="44"/>
       <c r="C14" s="18"/>
     </row>
   </sheetData>
@@ -6395,22 +6395,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>225</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:5" ht="86.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="41" t="s">
         <v>224</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
@@ -6532,8 +6532,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="42"/>
-      <c r="B10" s="42"/>
+      <c r="A10" s="44"/>
+      <c r="B10" s="44"/>
       <c r="C10" s="18"/>
       <c r="E10" s="2"/>
     </row>
@@ -6569,22 +6569,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>227</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="41" t="s">
         <v>226</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
@@ -6767,22 +6767,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>229</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:5" s="2" customFormat="1" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="41" t="s">
         <v>228</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
@@ -7035,26 +7035,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>181</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="58.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="28" t="s">
         <v>190</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
@@ -8186,26 +8186,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>188</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="50.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="30" t="s">
         <v>187</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="30"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="32"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
@@ -8513,26 +8513,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>159</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
     </row>
     <row r="2" spans="1:16" ht="46.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="30" t="s">
         <v>192</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="30"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="32"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
@@ -8843,26 +8843,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>186</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
     </row>
     <row r="2" spans="1:15" s="2" customFormat="1" ht="41.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="30" t="s">
         <v>191</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="30"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="32"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
@@ -9285,22 +9285,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="33" t="s">
         <v>189</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="35"/>
     </row>
     <row r="2" spans="1:5" s="2" customFormat="1" ht="37.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="30" t="s">
         <v>193</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="37"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
@@ -9516,22 +9516,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="35"/>
     </row>
     <row r="2" spans="1:5" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="30" t="s">
         <v>194</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="37"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
@@ -9662,26 +9662,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>196</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
     </row>
     <row r="2" spans="1:7" ht="43.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="30" t="s">
         <v>197</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="30"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="32"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
@@ -10069,7 +10069,7 @@
         <v>165</v>
       </c>
       <c r="E20" s="2"/>
-      <c r="F20" s="43">
+      <c r="F20" s="25">
         <v>8.3333333333333339</v>
       </c>
       <c r="G20" s="2"/>

</xml_diff>